<commit_message>
committing some more files and edits
</commit_message>
<xml_diff>
--- a/DevOps/DevOps_Tracker.xlsx
+++ b/DevOps/DevOps_Tracker.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="100">
   <si>
     <t>Building Maven Project</t>
   </si>
@@ -412,6 +412,10 @@
   <si>
     <t>About Logstash:
 https://www.elastic.co/guide/en/logstash/current/introduction.html</t>
+  </si>
+  <si>
+    <t>Getting Started with ElasticSearch:
+https://www.youtube.com/watch?v=60UsHHsKyN4</t>
   </si>
 </sst>
 </file>
@@ -896,10 +900,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -920,6 +924,11 @@
     <row r="3" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding more files to repo
</commit_message>
<xml_diff>
--- a/DevOps/DevOps_Tracker.xlsx
+++ b/DevOps/DevOps_Tracker.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="101">
   <si>
     <t>Building Maven Project</t>
   </si>
@@ -401,21 +401,26 @@
     <t>http://blog.flowdock.com/2014/11/11/chatops-devops-with-hubot/</t>
   </si>
   <si>
+    <t>Analytics with Kibana and Elasticsearch through Hadoop – part 1 – Introduction:
+http://www.rittmanmead.com/2014/11/analytics-with-kibana-and-elasticsearch-through-hadoop-part-1-introduction/</t>
+  </si>
+  <si>
+    <t>About Logstash:
+https://www.elastic.co/guide/en/logstash/current/introduction.html</t>
+  </si>
+  <si>
+    <t>Getting Started with ElasticSearch:
+https://www.youtube.com/watch?v=60UsHHsKyN4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demo on ElasticSearch, Logstash and Kibana (ELK):
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Demo on ElasticSearch, Logstash and Kibana (ELK):
 https://www.youtube.com/watch?v=Kqs7UcCJquM
+http://blog.webkid.io/visualize-datasets-with-elk/
 </t>
-  </si>
-  <si>
-    <t>Analytics with Kibana and Elasticsearch through Hadoop – part 1 – Introduction:
-http://www.rittmanmead.com/2014/11/analytics-with-kibana-and-elasticsearch-through-hadoop-part-1-introduction/</t>
-  </si>
-  <si>
-    <t>About Logstash:
-https://www.elastic.co/guide/en/logstash/current/introduction.html</t>
-  </si>
-  <si>
-    <t>Getting Started with ElasticSearch:
-https://www.youtube.com/watch?v=60UsHHsKyN4</t>
   </si>
 </sst>
 </file>
@@ -900,34 +905,37 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="16384" width="50.5546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edited DevOps Tracket sheet
</commit_message>
<xml_diff>
--- a/DevOps/DevOps_Tracker.xlsx
+++ b/DevOps/DevOps_Tracker.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="102">
   <si>
     <t>Building Maven Project</t>
   </si>
@@ -414,13 +414,18 @@
   </si>
   <si>
     <t xml:space="preserve">Demo on ElasticSearch, Logstash and Kibana (ELK):
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demo on ElasticSearch, Logstash and Kibana (ELK):
 https://www.youtube.com/watch?v=Kqs7UcCJquM
 http://blog.webkid.io/visualize-datasets-with-elk/
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logstash pitfalls to avoid those:
+http://logz.io/blog/5-logstash-pitfalls-and-how-to-avoid-them/
+</t>
+  </si>
+  <si>
+    <t>How preprocess logs with logstash:
+http://blog.mmlac.com/how-to-pre-process-logs-with-logstash/</t>
   </si>
 </sst>
 </file>
@@ -905,9 +910,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -916,7 +923,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="72" x14ac:dyDescent="0.3">
@@ -934,9 +941,14 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added daily status to Driver sheet
</commit_message>
<xml_diff>
--- a/DevOps/DevOps_Tracker.xlsx
+++ b/DevOps/DevOps_Tracker.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="103">
   <si>
     <t>Building Maven Project</t>
   </si>
@@ -426,6 +426,9 @@
   <si>
     <t>How preprocess logs with logstash:
 http://blog.mmlac.com/how-to-pre-process-logs-with-logstash/</t>
+  </si>
+  <si>
+    <t>http://tales.itnobody.com/2013/07/using-logstash-to-log-smtp-bounces-like-a-boss.html</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -486,6 +489,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -910,10 +916,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -951,9 +957,17 @@
         <v>101</v>
       </c>
     </row>
+    <row r="7" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A7" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Committing lot of updates
</commit_message>
<xml_diff>
--- a/DevOps/DevOps_Tracker.xlsx
+++ b/DevOps/DevOps_Tracker.xlsx
@@ -413,22 +413,23 @@
 https://www.youtube.com/watch?v=60UsHHsKyN4</t>
   </si>
   <si>
+    <t xml:space="preserve">Logstash pitfalls to avoid those:
+http://logz.io/blog/5-logstash-pitfalls-and-how-to-avoid-them/
+</t>
+  </si>
+  <si>
+    <t>How preprocess logs with logstash:
+http://blog.mmlac.com/how-to-pre-process-logs-with-logstash/</t>
+  </si>
+  <si>
+    <t>http://tales.itnobody.com/2013/07/using-logstash-to-log-smtp-bounces-like-a-boss.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">Demo on ElasticSearch, Logstash and Kibana (ELK):
 https://www.youtube.com/watch?v=Kqs7UcCJquM
 http://blog.webkid.io/visualize-datasets-with-elk/
+abc
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logstash pitfalls to avoid those:
-http://logz.io/blog/5-logstash-pitfalls-and-how-to-avoid-them/
-</t>
-  </si>
-  <si>
-    <t>How preprocess logs with logstash:
-http://blog.mmlac.com/how-to-pre-process-logs-with-logstash/</t>
-  </si>
-  <si>
-    <t>http://tales.itnobody.com/2013/07/using-logstash-to-log-smtp-bounces-like-a-boss.html</t>
   </si>
 </sst>
 </file>
@@ -918,18 +919,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="16384" width="50.5546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="72" x14ac:dyDescent="0.3">
@@ -949,17 +948,17 @@
     </row>
     <row r="5" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating daily status in Driver sheet
</commit_message>
<xml_diff>
--- a/DevOps/DevOps_Tracker.xlsx
+++ b/DevOps/DevOps_Tracker.xlsx
@@ -428,7 +428,6 @@
     <t xml:space="preserve">Demo on ElasticSearch, Logstash and Kibana (ELK):
 https://www.youtube.com/watch?v=Kqs7UcCJquM
 http://blog.webkid.io/visualize-datasets-with-elk/
-abc
 </t>
   </si>
 </sst>
@@ -919,7 +918,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>